<commit_message>
Final Project week2 summary
</commit_message>
<xml_diff>
--- a/Expected time.xlsx
+++ b/Expected time.xlsx
@@ -11,27 +11,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
-  <si>
-    <t>Ball Path Task</t>
-  </si>
-  <si>
-    <t>4 days</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+  <si>
+    <t>Btn handler task</t>
+  </si>
+  <si>
+    <t>1 week</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
   <si>
     <t>Platform diraction task</t>
   </si>
   <si>
+    <t>not done</t>
+  </si>
+  <si>
     <t>physics task</t>
   </si>
   <si>
-    <t>2 weeks</t>
-  </si>
-  <si>
     <t>LCD display task</t>
-  </si>
-  <si>
-    <t>1 week</t>
   </si>
   <si>
     <t>LED display task</t>
@@ -46,10 +46,12 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -299,29 +301,41 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -329,7 +343,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>